<commit_message>
fix problem with selection of arguments
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>№</t>
   </si>
@@ -179,7 +179,17 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -192,6 +202,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -242,6 +272,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -257,6 +307,76 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -577,19 +697,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="64.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -599,8 +719,11 @@
       <c r="C1" s="1">
         <v>41379</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1">
+        <v>41380</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -611,7 +734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -622,7 +745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -633,7 +756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -643,8 +766,11 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -655,7 +781,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -666,7 +792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -677,7 +803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -688,7 +814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -699,7 +825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -710,27 +836,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -762,16 +888,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:Z43">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"NG"</formula>
+      <formula>"OK"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"?"</formula>

</xml_diff>

<commit_message>
fix problem in page loading
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>№</t>
   </si>
@@ -700,12 +700,12 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="64.7109375" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
     <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -744,6 +744,9 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -834,6 +837,9 @@
       </c>
       <c r="C11" t="s">
         <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
check warnings, fix counters update
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>№</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>не переименовываются вызовы функций при переимновании определений</t>
-  </si>
-  <si>
-    <t>проблемы с преобразованием кода в команды</t>
-  </si>
-  <si>
-    <t>аргументы функций</t>
   </si>
   <si>
     <t>при загрузке задач на первой вкладке рисуются сосуды</t>
@@ -133,6 +127,12 @@
   </si>
   <si>
     <t>"NetworkError: 404 Not Found - http://localhost/courseWork/ev/jquery.js"</t>
+  </si>
+  <si>
+    <t>получили из команд некорректный код, не теряем команды при возврате</t>
+  </si>
+  <si>
+    <t>при пошаговом выполнении в визуальном режиме криво обновляются каунтеры</t>
   </si>
 </sst>
 </file>
@@ -242,31 +242,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -697,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,6 +733,9 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -742,10 +745,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -753,10 +756,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -767,10 +773,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -781,7 +787,10 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -792,18 +801,24 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -811,21 +826,27 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -835,11 +856,8 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -877,47 +895,32 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+  <conditionalFormatting sqref="C2:C9">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:Z41">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"?"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:Z43">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"NG"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"?"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
block interface during commands execution
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>№</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>submit isn't defined</t>
+  </si>
+  <si>
+    <t>не обнуляется состояние, если дошли до какого-то шага и уменьшили каунтер</t>
+  </si>
+  <si>
+    <t>добавили forward, выполнили частично, преобразовали в код, когда обратно -- ошибка</t>
   </si>
 </sst>
 </file>
@@ -700,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,11 +884,23 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -897,11 +915,6 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -921,7 +934,7 @@
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:Z41">
+  <conditionalFormatting sqref="C2:Z40">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix continue of commands execution
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>№</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>добавили forward, выполнили частично, преобразовали в код, когда обратно -- ошибка</t>
+  </si>
+  <si>
+    <t>выполнили команду, увеличили каунтер, поставили плей -- ничего не меняется</t>
+  </si>
+  <si>
+    <t>повтор, внутри команда. Если увеличиваем каунтер у команды, не сбрасывается текущая команда</t>
+  </si>
+  <si>
+    <t>повтор, внутри команда. Если увеличиваем каунтер у повтора сбрасывается текущая команда</t>
   </si>
 </sst>
 </file>
@@ -188,7 +197,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -246,156 +255,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -706,19 +565,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -731,8 +590,11 @@
       <c r="D1" s="1">
         <v>41380</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1">
+        <v>41381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -746,7 +608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -760,7 +622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -774,7 +636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -788,7 +650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -802,7 +664,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -816,7 +678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -830,7 +692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -844,7 +706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -858,7 +720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -869,7 +731,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -880,7 +742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -890,8 +752,11 @@
       <c r="D13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -902,19 +767,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix for statements comparing
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>№</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>повтор, внутри команда. Если увеличиваем каунтер у повтора сбрасывается текущая команда</t>
+  </si>
+  <si>
+    <t>криво показывается каунтер у повтора: I вместо i/j</t>
+  </si>
+  <si>
+    <t>выполнили команду, увеличили каунтер -- выполняется, но кривой каунтер</t>
   </si>
 </sst>
 </file>
@@ -565,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +803,84 @@
         <v>20</v>
       </c>
       <c r="E17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix comparing of statements, fix for counter
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>№</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>выполнили команду, увеличили каунтер -- выполняется, но кривой каунтер</t>
+  </si>
+  <si>
+    <t>остаются подвеченными каунтеры</t>
   </si>
 </sst>
 </file>
@@ -574,7 +577,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,6 +714,9 @@
       <c r="D9" t="s">
         <v>9</v>
       </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -792,7 +798,7 @@
         <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -814,7 +820,7 @@
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -831,6 +837,12 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
properly update for statement counter on start of playing
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>№</t>
   </si>
@@ -159,7 +159,13 @@
     <t>выполнили команду, увеличили каунтер -- выполняется, но кривой каунтер</t>
   </si>
   <si>
-    <t>остаются подвеченными каунтеры</t>
+    <t>остаются подвеченными каунтеры в повторе</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Как только вошли в тело цикла второй раз, некорректно отображается каунтер у повтора при переходе на один шаг назад:
+for i in range(2):
+  forward(2)
+</t>
   </si>
 </sst>
 </file>
@@ -576,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,9 +851,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix highlighting of for statement
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -583,7 +583,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +848,7 @@
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix updation of counters in command
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -583,7 +583,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,7 +837,7 @@
         <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix counter updation in for statement
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +859,7 @@
         <v>24</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update test results, 2 new bugs has been found
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
   <si>
     <t>№</t>
   </si>
@@ -129,9 +129,6 @@
     <t>"NetworkError: 404 Not Found - http://localhost/courseWork/ev/jquery.js"</t>
   </si>
   <si>
-    <t>получили из команд некорректный код, не теряем команды при возврате</t>
-  </si>
-  <si>
     <t>при пошаговом выполнении в визуальном режиме криво обновляются каунтеры</t>
   </si>
   <si>
@@ -166,6 +163,12 @@
 for i in range(2):
   forward(2)
 </t>
+  </si>
+  <si>
+    <t>При удалении аргументов из определения, не удаляются из вызовов =&gt; проблемы при переименовании и вообще всех операциях</t>
+  </si>
+  <si>
+    <t>получили из команд некорректный код, не теряем команды при возврате: потеряли функцию</t>
   </si>
 </sst>
 </file>
@@ -582,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,6 +639,9 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -650,6 +656,9 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -664,6 +673,9 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -678,6 +690,9 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -692,8 +707,11 @@
       <c r="D7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -704,6 +722,9 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -729,13 +750,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -743,9 +767,12 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -754,9 +781,12 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -765,7 +795,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -779,9 +809,12 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -790,7 +823,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
@@ -801,7 +834,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
@@ -812,7 +845,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
@@ -823,7 +856,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
@@ -834,7 +867,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
@@ -845,7 +878,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
         <v>9</v>
@@ -856,7 +889,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
         <v>9</v>
@@ -865,6 +898,12 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
don't remove commands on converting to code
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
   <si>
     <t>№</t>
   </si>
@@ -583,19 +583,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -611,8 +611,11 @@
       <c r="E1" s="1">
         <v>41381</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1">
+        <v>41382</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -626,7 +629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -643,7 +646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -660,7 +663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -677,7 +680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -694,7 +697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -711,7 +714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -728,7 +731,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -745,7 +748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -761,8 +764,11 @@
       <c r="E10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -776,7 +782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -790,7 +796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -804,7 +810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -818,7 +824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -829,7 +835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
properly remove function call arguments of removing arguments in function definition
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -586,7 +586,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +909,7 @@
         <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix stuck on  adding several arguments in function
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
   <si>
     <t>№</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>получили из команд некорректный код, не теряем команды при возврате: потеряли функцию</t>
+  </si>
+  <si>
+    <t>Добавили функцию, ее вызов, добавили аргумент, удалили, добавили, пытаемся еще добавить - виснет</t>
   </si>
 </sst>
 </file>
@@ -585,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -857,7 +860,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -868,7 +871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -879,7 +882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -890,7 +893,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -901,7 +904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -912,42 +915,48 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
properly convert condiiton arguments from code to visual representation
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="29">
   <si>
     <t>№</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>Добавили функцию, ее вызов, добавили аргумент, удалили, добавили, пытаемся еще добавить - виснет</t>
+  </si>
+  <si>
+    <t>Тормозит выполнение первой команды в пошаговом режиме</t>
+  </si>
+  <si>
+    <t>При преобразовании кода условий в команды не учитывается  сравнивающая функция</t>
   </si>
 </sst>
 </file>
@@ -588,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,8 +654,11 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -663,6 +672,9 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -682,6 +694,9 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -699,6 +714,9 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -716,8 +734,11 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -731,6 +752,9 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -750,6 +774,9 @@
       <c r="E9" t="s">
         <v>9</v>
       </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -784,6 +811,9 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -798,6 +828,9 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -812,6 +845,9 @@
       <c r="E13" t="s">
         <v>9</v>
       </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -826,6 +862,9 @@
       <c r="E14" t="s">
         <v>9</v>
       </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -837,6 +876,9 @@
       <c r="E15" t="s">
         <v>9</v>
       </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -848,6 +890,9 @@
       <c r="E16" t="s">
         <v>9</v>
       </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -859,6 +904,9 @@
       <c r="E17" t="s">
         <v>9</v>
       </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -870,6 +918,9 @@
       <c r="E18" t="s">
         <v>9</v>
       </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -881,6 +932,9 @@
       <c r="E19" t="s">
         <v>9</v>
       </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -892,6 +946,9 @@
       <c r="E20" t="s">
         <v>9</v>
       </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -903,6 +960,9 @@
       <c r="E21" t="s">
         <v>9</v>
       </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -914,6 +974,9 @@
       <c r="E22" t="s">
         <v>9</v>
       </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -930,10 +993,22 @@
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix commands with several arguments
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
   <si>
     <t>№</t>
   </si>
@@ -174,10 +174,25 @@
     <t>Добавили функцию, ее вызов, добавили аргумент, удалили, добавили, пытаемся еще добавить - виснет</t>
   </si>
   <si>
-    <t>Тормозит выполнение первой команды в пошаговом режиме</t>
-  </si>
-  <si>
     <t>При преобразовании кода условий в команды не учитывается  сравнивающая функция</t>
+  </si>
+  <si>
+    <t>Can't decrease not int!!!
+pour(1, 2)
+pourOut(2)
+pour(1, 2)
+pourOut(2)
+pour(1, 2)
+pourOut(2)</t>
+  </si>
+  <si>
+    <t>Неправильные аргументы у переливания</t>
+  </si>
+  <si>
+    <t>Прятать сосуды при переключении на первую вкладку</t>
+  </si>
+  <si>
+    <t>unhadled error при отправке решений с переливанием</t>
   </si>
 </sst>
 </file>
@@ -592,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,14 +1012,14 @@
         <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F25" t="s">
@@ -1015,25 +1030,38 @@
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1053,7 +1081,7 @@
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:Z40">
+  <conditionalFormatting sqref="C2:Z39">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>

</xml_diff>

<commit_message>
don't draw vessels on the firts tab
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="35">
   <si>
     <t>№</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>для переливания посылаем код, в котором какое-то из промежуточных состояний -- выигрышное, но конечное -- нет</t>
+  </si>
+  <si>
+    <t>передача пустого аргумента в функцию, выбор его в селекте</t>
+  </si>
+  <si>
+    <t>передача некорректного аргумента в каунтер</t>
   </si>
 </sst>
 </file>
@@ -610,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,6 +684,9 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -698,6 +707,9 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -718,6 +730,9 @@
       <c r="F5" t="s">
         <v>9</v>
       </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1053,6 +1068,9 @@
       <c r="F27" t="s">
         <v>8</v>
       </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1077,6 +1095,87 @@
       </c>
       <c r="G29" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix showing of command arguments
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="41">
   <si>
     <t>№</t>
   </si>
@@ -202,6 +202,36 @@
   </si>
   <si>
     <t>передача некорректного аргумента в каунтер</t>
+  </si>
+  <si>
+    <t>названия функций для сравнения должны быть на русском</t>
+  </si>
+  <si>
+    <t>положение кнопки у spin</t>
+  </si>
+  <si>
+    <t>перевести сообщения об ошибках</t>
+  </si>
+  <si>
+    <t xml:space="preserve">криво выводится каунтер у команды
+def func0(arg0):
+  if objectPosition("wall", "atTheLeft"):
+    forward(arg0)
+func0(2)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def func0(arg0, arg1):
+  forward(arg0)
+  forward(1)
+func0(2, 1)
+</t>
+  </si>
+  <si>
+    <t>def func0(arg0, arg1):
+  forward(arg0)
+  forward(arg1)
+func0(2, 1)</t>
   </si>
 </sst>
 </file>
@@ -618,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,6 +783,9 @@
       <c r="F6" t="s">
         <v>9</v>
       </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -773,6 +806,9 @@
       <c r="F7" t="s">
         <v>9</v>
       </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -793,6 +829,9 @@
       <c r="F8" t="s">
         <v>9</v>
       </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -813,6 +852,9 @@
       <c r="F9" t="s">
         <v>9</v>
       </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -831,6 +873,9 @@
         <v>8</v>
       </c>
       <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -850,6 +895,9 @@
       <c r="F11" t="s">
         <v>9</v>
       </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -867,6 +915,9 @@
       <c r="F12" t="s">
         <v>9</v>
       </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -884,6 +935,9 @@
       <c r="F13" t="s">
         <v>9</v>
       </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -901,6 +955,9 @@
       <c r="F14" t="s">
         <v>9</v>
       </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -915,6 +972,9 @@
       <c r="F15" t="s">
         <v>9</v>
       </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -929,6 +989,9 @@
       <c r="F16" t="s">
         <v>9</v>
       </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -943,6 +1006,9 @@
       <c r="F17" t="s">
         <v>9</v>
       </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -957,6 +1023,9 @@
       <c r="F18" t="s">
         <v>9</v>
       </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -971,6 +1040,9 @@
       <c r="F19" t="s">
         <v>9</v>
       </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -985,6 +1057,9 @@
       <c r="F20" t="s">
         <v>9</v>
       </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -999,6 +1074,9 @@
       <c r="F21" t="s">
         <v>9</v>
       </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1013,6 +1091,9 @@
       <c r="F22" t="s">
         <v>9</v>
       </c>
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1024,6 +1105,9 @@
       <c r="F23" t="s">
         <v>9</v>
       </c>
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1035,6 +1119,9 @@
       <c r="F24" t="s">
         <v>9</v>
       </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1046,6 +1133,9 @@
       <c r="F25" t="s">
         <v>9</v>
       </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1057,6 +1147,9 @@
       <c r="F26" t="s">
         <v>9</v>
       </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1104,6 +1197,9 @@
       <c r="B30" t="s">
         <v>33</v>
       </c>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1112,68 +1208,107 @@
       <c r="B31" t="s">
         <v>34</v>
       </c>
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1207,6 +1342,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1226,7 +1362,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
add russian titles of codition functions
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="41">
   <si>
     <t>№</t>
   </si>
@@ -646,19 +646,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -680,8 +680,11 @@
       <c r="G1" s="1">
         <v>41384</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1">
+        <v>41385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -695,7 +698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -718,7 +721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -741,7 +744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -764,7 +767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -787,7 +790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -810,7 +813,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -833,7 +836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -856,7 +859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -879,7 +882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -899,7 +902,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -919,7 +922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -939,7 +942,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -959,7 +962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -976,7 +979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -993,7 +996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1095,7 +1098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1109,7 +1112,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1165,7 +1168,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1190,7 +1193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1222,8 +1225,11 @@
       <c r="G32" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1233,8 +1239,11 @@
       <c r="G33" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1245,7 +1254,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1256,7 +1265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1267,7 +1276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1278,37 +1287,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
translate all eror messages in russian
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="41">
   <si>
     <t>№</t>
   </si>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,6 +1252,9 @@
       </c>
       <c r="G34" t="s">
         <v>8</v>
+      </c>
+      <c r="H34" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix for statement body highlighting
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="43">
   <si>
     <t>№</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>криво подсвечивается текущая команда</t>
+  </si>
+  <si>
+    <t>повтор, подсвечивается все тело</t>
   </si>
 </sst>
 </file>
@@ -651,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,6 +726,9 @@
       <c r="G3" t="s">
         <v>9</v>
       </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -746,6 +752,9 @@
       <c r="G4" t="s">
         <v>9</v>
       </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -769,6 +778,9 @@
       <c r="G5" t="s">
         <v>9</v>
       </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -792,6 +804,9 @@
       <c r="G6" t="s">
         <v>9</v>
       </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -815,6 +830,9 @@
       <c r="G7" t="s">
         <v>9</v>
       </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -838,6 +856,9 @@
       <c r="G8" t="s">
         <v>9</v>
       </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -861,6 +882,9 @@
       <c r="G9" t="s">
         <v>9</v>
       </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -882,6 +906,9 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -904,6 +931,9 @@
       <c r="G11" t="s">
         <v>9</v>
       </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -924,8 +954,11 @@
       <c r="G12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -942,6 +975,9 @@
         <v>9</v>
       </c>
       <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -964,6 +1000,9 @@
       <c r="G14" t="s">
         <v>9</v>
       </c>
+      <c r="H14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -981,6 +1020,9 @@
       <c r="G15" t="s">
         <v>9</v>
       </c>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -998,6 +1040,9 @@
       <c r="G16" t="s">
         <v>9</v>
       </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -1015,6 +1060,9 @@
       <c r="G17" t="s">
         <v>9</v>
       </c>
+      <c r="H17" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1032,6 +1080,9 @@
       <c r="G18" t="s">
         <v>9</v>
       </c>
+      <c r="H18" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1049,6 +1100,9 @@
       <c r="G19" t="s">
         <v>9</v>
       </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1066,6 +1120,9 @@
       <c r="G20" t="s">
         <v>9</v>
       </c>
+      <c r="H20" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1083,6 +1140,9 @@
       <c r="G21" t="s">
         <v>9</v>
       </c>
+      <c r="H21" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1100,6 +1160,9 @@
       <c r="G22" t="s">
         <v>9</v>
       </c>
+      <c r="H22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1114,6 +1177,9 @@
       <c r="G23" t="s">
         <v>9</v>
       </c>
+      <c r="H23" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1128,6 +1194,9 @@
       <c r="G24" t="s">
         <v>9</v>
       </c>
+      <c r="H24" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1142,6 +1211,9 @@
       <c r="G25" t="s">
         <v>9</v>
       </c>
+      <c r="H25" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1156,6 +1228,9 @@
       <c r="G26" t="s">
         <v>9</v>
       </c>
+      <c r="H26" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1170,6 +1245,9 @@
       <c r="G27" t="s">
         <v>9</v>
       </c>
+      <c r="H27" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1184,6 +1262,9 @@
       <c r="G28" t="s">
         <v>9</v>
       </c>
+      <c r="H28" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -1195,6 +1276,9 @@
       <c r="G29" t="s">
         <v>9</v>
       </c>
+      <c r="H29" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -1206,6 +1290,9 @@
       <c r="G30" t="s">
         <v>9</v>
       </c>
+      <c r="H30" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1217,6 +1304,9 @@
       <c r="G31" t="s">
         <v>9</v>
       </c>
+      <c r="H31" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -1270,6 +1360,9 @@
       <c r="G35" t="s">
         <v>9</v>
       </c>
+      <c r="H35" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
@@ -1281,6 +1374,9 @@
       <c r="G36" t="s">
         <v>9</v>
       </c>
+      <c r="H36" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
@@ -1292,6 +1388,9 @@
       <c r="G37" t="s">
         <v>9</v>
       </c>
+      <c r="H37" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
@@ -1307,6 +1406,12 @@
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
proper count points for pourer
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="44">
   <si>
     <t>№</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>повтор, подсвечивается все тело</t>
+  </si>
+  <si>
+    <t>неправильно считается количество очков для переливания</t>
   </si>
 </sst>
 </file>
@@ -284,7 +287,37 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -654,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,6 +1451,12 @@
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H40" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -1441,29 +1480,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C9">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:Z39">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="C2:Z39 H40">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix points computation in code mode
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -720,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,7 +1499,7 @@
         <v>44</v>
       </c>
       <c r="H41" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
stop execution on code changes
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="47">
   <si>
     <t>№</t>
   </si>
@@ -245,6 +245,12 @@
   <si>
     <t>неправильно считается количество очков для переливания в режиме кода</t>
   </si>
+  <si>
+    <t>при изменении кода сбрасывать выполнение команд</t>
+  </si>
+  <si>
+    <t>подписи для сосудов под границей</t>
+  </si>
 </sst>
 </file>
 
@@ -260,12 +266,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -280,17 +292,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -313,6 +326,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -323,6 +366,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -333,6 +386,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -343,11 +406,71 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -718,19 +841,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -755,8 +878,11 @@
       <c r="H1" s="1">
         <v>41385</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1">
+        <v>41386</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -770,7 +896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -796,7 +922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -822,7 +948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -848,7 +974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -874,7 +1000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -900,7 +1026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -926,7 +1052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -952,7 +1078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -978,7 +1104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1001,7 +1127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1024,7 +1150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1047,7 +1173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1070,7 +1196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1090,7 +1216,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1388,7 +1514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1402,7 +1528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1416,7 +1542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1430,7 +1556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1444,7 +1570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1458,7 +1584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1469,7 +1595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1480,7 +1606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1491,7 +1617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1502,47 +1628,67 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C9">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:Z39 H40:H41">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
-      <formula>"?"</formula>
+      <formula>"OK"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:Y355">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:Z39 H40:H41">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
-      <formula>"?"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
-      <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add WA for convertion arguments from code to visual mode
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="50">
   <si>
     <t>№</t>
   </si>
@@ -250,6 +250,38 @@
   </si>
   <si>
     <t>подписи для сосудов под границей</t>
+  </si>
+  <si>
+    <t>применять изменения имен функций и аргументов на Enter</t>
+  </si>
+  <si>
+    <t>Некорректный аргумент
+def func0(arg0):
+  if compare(2, "!=", arg0):
+    if checkFilled(1, "&gt;", 2):
+      sub(1, 2, arg0)
+    else:
+      sub(2, 1, arg0)
+def sub(arg0, arg1, arg2):
+  pour(arg0, arg1)
+  if compare(arg1, "!=", arg2):
+    pourOut(arg1)
+func0(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">не конвертируется в команды
+def func0(arg0):
+  if compare(2, "!=", arg0):
+    if checkFilled(1, "&gt;", 2):
+      sub(1, 2, arg0)
+    else:
+      sub(2, 1, arg0)
+def sub(arg0, arg1, arg2):
+  pour(arg0, arg1)
+  if compare(arg1, "!=", arg2):
+    pourOut(arg1)
+func0(5)
+</t>
   </si>
 </sst>
 </file>
@@ -841,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,6 +1685,84 @@
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add W/A for the problem with function definition removing
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="49">
   <si>
     <t>№</t>
   </si>
@@ -720,20 +720,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="71.7109375" customWidth="1"/>
     <col min="3" max="9" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -764,8 +764,11 @@
       <c r="J1" s="1">
         <v>41387</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1">
+        <v>41388</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -781,8 +784,11 @@
       <c r="J2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -811,7 +817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -840,7 +846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -869,7 +875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -898,7 +904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -927,7 +933,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -956,7 +962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -985,7 +991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1040,7 +1046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1066,7 +1072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1092,7 +1098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1118,7 +1124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1141,7 +1147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
fix looping in code execution when there is a bug in code
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="52">
   <si>
     <t>№</t>
   </si>
@@ -279,6 +279,20 @@
     pourOut(arg1)
 func0(5)
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NameError: name 'aaa' is not defined зацикливается
+def func0(arg0):
+  if compare(1, "&lt;", arg0):
+    pour(1, 2)
+func0(aaa)
+</t>
+  </si>
+  <si>
+    <t>подставлять значения аргументов в каунтеры и селекты? Опасно!!!</t>
+  </si>
+  <si>
+    <t>добавить возможность добавлять в роли аргументов строки, которыеи могут быть именаим переменных???</t>
   </si>
 </sst>
 </file>
@@ -332,7 +346,217 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -723,7 +947,7 @@
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,6 +1040,9 @@
       <c r="J3" t="s">
         <v>9</v>
       </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -845,6 +1072,9 @@
       <c r="J4" t="s">
         <v>9</v>
       </c>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -874,6 +1104,9 @@
       <c r="J5" t="s">
         <v>9</v>
       </c>
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -903,6 +1136,9 @@
       <c r="J6" t="s">
         <v>9</v>
       </c>
+      <c r="K6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -932,6 +1168,9 @@
       <c r="J7" t="s">
         <v>9</v>
       </c>
+      <c r="K7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -961,6 +1200,9 @@
       <c r="J8" t="s">
         <v>9</v>
       </c>
+      <c r="K8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -990,6 +1232,9 @@
       <c r="J9" t="s">
         <v>9</v>
       </c>
+      <c r="K9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1017,6 +1262,9 @@
         <v>9</v>
       </c>
       <c r="J10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1045,6 +1293,9 @@
       <c r="J11" t="s">
         <v>9</v>
       </c>
+      <c r="K11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1071,6 +1322,9 @@
       <c r="J12" t="s">
         <v>9</v>
       </c>
+      <c r="K12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1097,6 +1351,9 @@
       <c r="J13" t="s">
         <v>9</v>
       </c>
+      <c r="K13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1123,6 +1380,9 @@
       <c r="J14" t="s">
         <v>9</v>
       </c>
+      <c r="K14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1146,6 +1406,9 @@
       <c r="J15" t="s">
         <v>9</v>
       </c>
+      <c r="K15" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1169,8 +1432,11 @@
       <c r="J16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1192,8 +1458,11 @@
       <c r="J17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1215,8 +1484,11 @@
       <c r="J18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1238,8 +1510,11 @@
       <c r="J19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1261,8 +1536,11 @@
       <c r="J20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1284,8 +1562,11 @@
       <c r="J21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1307,8 +1588,11 @@
       <c r="J22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1327,8 +1611,11 @@
       <c r="J23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1347,8 +1634,11 @@
       <c r="J24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1367,8 +1657,11 @@
       <c r="J25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1387,8 +1680,11 @@
       <c r="J26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1407,8 +1703,11 @@
       <c r="J27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1427,8 +1726,11 @@
       <c r="J28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1444,8 +1746,11 @@
       <c r="J29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1461,8 +1766,11 @@
       <c r="J30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1478,8 +1786,11 @@
       <c r="J31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1495,8 +1806,11 @@
       <c r="J32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1512,8 +1826,11 @@
       <c r="J33" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1529,8 +1846,11 @@
       <c r="J34" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1546,8 +1866,11 @@
       <c r="J35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1563,8 +1886,11 @@
       <c r="J36" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1580,8 +1906,11 @@
       <c r="J37" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1594,8 +1923,11 @@
       <c r="J38" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1608,8 +1940,11 @@
       <c r="J39" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1622,8 +1957,11 @@
       <c r="J40" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1636,8 +1974,11 @@
       <c r="J41" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1650,8 +1991,11 @@
       <c r="J42" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1664,8 +2008,11 @@
       <c r="J43" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1678,8 +2025,11 @@
       <c r="J44" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
@@ -1692,20 +2042,41 @@
       <c r="J45" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K48" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
@@ -1745,38 +2116,48 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C9">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:Z39 H40:H41">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:Y354">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"NG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix commands highlighting and while initialization
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="54">
   <si>
     <t>№</t>
   </si>
@@ -301,6 +301,21 @@
 def func1():
   func1()
 func1()
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">криво инициализируетсят while:
+def func0():
+  while objectPosition("wall", "atTheLeft"):
+    forward(1)
+for i in range(3):
+  forward(4)
+forward(1)
+func0()
+if objectPosition("wall", "atTheLeft"):
+  forward(1)
+else:
+  forward(1)
 </t>
   </si>
 </sst>
@@ -765,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,6 +953,9 @@
       <c r="K5" t="s">
         <v>9</v>
       </c>
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -970,6 +988,9 @@
       <c r="K6" t="s">
         <v>9</v>
       </c>
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1002,6 +1023,9 @@
       <c r="K7" t="s">
         <v>9</v>
       </c>
+      <c r="L7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1034,6 +1058,9 @@
       <c r="K8" t="s">
         <v>9</v>
       </c>
+      <c r="L8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1066,6 +1093,9 @@
       <c r="K9" t="s">
         <v>9</v>
       </c>
+      <c r="L9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1096,6 +1126,9 @@
         <v>9</v>
       </c>
       <c r="K10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1127,6 +1160,9 @@
       <c r="K11" t="s">
         <v>9</v>
       </c>
+      <c r="L11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1185,6 +1221,9 @@
       <c r="K13" t="s">
         <v>9</v>
       </c>
+      <c r="L13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1214,6 +1253,9 @@
       <c r="K14" t="s">
         <v>9</v>
       </c>
+      <c r="L14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1240,6 +1282,9 @@
       <c r="K15" t="s">
         <v>9</v>
       </c>
+      <c r="L15" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1266,8 +1311,11 @@
       <c r="K16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1292,8 +1340,11 @@
       <c r="K17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1318,8 +1369,11 @@
       <c r="K18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1344,8 +1398,11 @@
       <c r="K19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1370,8 +1427,11 @@
       <c r="K20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1396,8 +1456,11 @@
       <c r="K21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1422,8 +1485,11 @@
       <c r="K22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1445,8 +1511,11 @@
       <c r="K23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1469,7 +1538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1492,7 +1561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1515,7 +1584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1538,7 +1607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1561,7 +1630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1581,7 +1650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1601,7 +1670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1621,7 +1690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1921,9 +1990,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L50" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix arguments in for
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="55">
   <si>
     <t>№</t>
   </si>
@@ -316,6 +316,26 @@
   forward(1)
 else:
   forward(1)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">не конвертируются аргументы функции в каунтере фора:
+def moveForward():
+  while not objectPosition("wall", "inFrontOf"):
+    forward(1)
+def rotate():
+  if objectPosition("wall", "atTheRight"):
+    left(1)
+  else:
+    right(1)
+def solve(arg0):
+  for i in range(arg0):
+    moveForward()
+    rotate()
+solve(41)
+forward(1)
+right(1)
+solve(32)
 </t>
   </si>
 </sst>
@@ -780,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,6 +2022,9 @@
       <c r="K45" t="s">
         <v>9</v>
       </c>
+      <c r="L45" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
@@ -2013,6 +2036,9 @@
       <c r="K46" t="s">
         <v>9</v>
       </c>
+      <c r="L46" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -2058,9 +2084,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="285" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L51" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update test results, add new tests
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="64">
   <si>
     <t>№</t>
   </si>
@@ -319,6 +319,17 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">конвертация, выполнение def func0(arg0):
+  if objectPosition("cell", "inFrontOf"):
+    forward(1)
+    func0(2)
+func0(1)
+</t>
+  </si>
+  <si>
+    <t>ошибка при вводе корректного каунтера с клавиатуры</t>
+  </si>
+  <si>
     <t xml:space="preserve">не конвертируются аргументы функции в каунтере фора:
 def moveForward():
   while not objectPosition("wall", "inFrontOf"):
@@ -339,12 +350,47 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">конвертация, выполнение def func0(arg0):
-  if objectPosition("cell", "inFrontOf"):
+    <t>в селекте не выбираются аргументы</t>
+  </si>
+  <si>
+    <t>is blocked by #54</t>
+  </si>
+  <si>
+    <t>need to add name or number</t>
+  </si>
+  <si>
+    <t>Некорректно конвертируются условия в команды 
+def func0(arg0):
+  if compare(2, "!=", arg0):
+    if checkFilled(1, "&gt;", 2):
+      sub(1, 2, arg0)
+    else:
+      sub(2, 1, arg0)
+def sub(arg0, arg1, arg2):
+  pour(arg0, arg1)
+  if compare(arg1, "!=", arg2):
+    pourOut(arg1)
+func0(5)</t>
+  </si>
+  <si>
+    <t>is blocked by#55</t>
+  </si>
+  <si>
+    <t>Не конвертируется в команды, TypeError: (intermediate value).dict is undefined
+def func0():
+  while objectPosition("wall", "atTheLeft"):
     forward(1)
-    func0(2)
-func0(1)
-</t>
+for i in range(3):
+  forward(4)
+forward(1)
+func0()
+if objectPosition("wall", "atTheLeft"):
+  forward(1)
+else:
+  forward(1)</t>
+  </si>
+  <si>
+    <t>is  blocked by #56</t>
   </si>
 </sst>
 </file>
@@ -361,7 +407,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +417,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,18 +439,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -806,20 +879,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="9" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -856,8 +929,11 @@
       <c r="L1" s="1">
         <v>41389</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="1">
+        <v>41407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -879,8 +955,11 @@
       <c r="L2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -914,8 +993,11 @@
       <c r="L3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -949,8 +1031,11 @@
       <c r="L4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -984,8 +1069,11 @@
       <c r="L5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1019,8 +1107,11 @@
       <c r="L6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1054,8 +1145,11 @@
       <c r="L7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1089,8 +1183,11 @@
       <c r="L8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1124,8 +1221,11 @@
       <c r="L9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1159,8 +1259,11 @@
       <c r="L10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1191,8 +1294,11 @@
       <c r="L11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1221,7 +1327,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1252,8 +1358,11 @@
       <c r="L13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1284,8 +1393,11 @@
       <c r="L14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1313,8 +1425,11 @@
       <c r="L15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1342,8 +1457,11 @@
       <c r="L16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1371,8 +1489,11 @@
       <c r="L17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1400,8 +1521,11 @@
       <c r="L18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1429,8 +1553,11 @@
       <c r="L19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1458,8 +1585,11 @@
       <c r="L20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1487,8 +1617,11 @@
       <c r="L21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1516,8 +1649,11 @@
       <c r="L22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1542,8 +1678,11 @@
       <c r="L23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1568,8 +1707,11 @@
       <c r="L24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1594,8 +1736,11 @@
       <c r="L25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1620,8 +1765,11 @@
       <c r="L26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1646,8 +1794,11 @@
       <c r="L27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1670,7 +1821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1689,8 +1840,11 @@
       <c r="K29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1712,8 +1866,14 @@
       <c r="L30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1735,8 +1895,11 @@
       <c r="L31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1758,8 +1921,11 @@
       <c r="L32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1781,8 +1947,11 @@
       <c r="L33" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1804,8 +1973,11 @@
       <c r="L34" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1827,8 +1999,11 @@
       <c r="L35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1850,8 +2025,11 @@
       <c r="L36" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1873,8 +2051,11 @@
       <c r="L37" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1893,8 +2074,11 @@
       <c r="L38" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1913,8 +2097,11 @@
       <c r="L39" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1933,8 +2120,11 @@
       <c r="L40" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1953,8 +2143,11 @@
       <c r="L41" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1973,8 +2166,11 @@
       <c r="L42" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1993,8 +2189,14 @@
       <c r="L43" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
+        <v>8</v>
+      </c>
+      <c r="N43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2013,8 +2215,14 @@
       <c r="L44" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M44" t="s">
+        <v>8</v>
+      </c>
+      <c r="N44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
@@ -2033,8 +2241,11 @@
       <c r="L45" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
@@ -2047,8 +2258,11 @@
       <c r="L46" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
@@ -2059,7 +2273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
       </c>
@@ -2070,7 +2284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>49</v>
       </c>
@@ -2080,8 +2294,11 @@
       <c r="L49" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+      <c r="M49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
@@ -2091,84 +2308,363 @@
       <c r="L50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="285" x14ac:dyDescent="0.25">
+      <c r="M50" t="s">
+        <v>8</v>
+      </c>
+      <c r="N50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L51" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="M51" t="s">
+        <v>8</v>
+      </c>
+      <c r="N51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>52</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="M52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
+      <c r="B55" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C9">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:Z39 H40:H41">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:Y354">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
return the result of the function's execution in FuncDef.executeBody()
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="64">
   <si>
     <t>№</t>
   </si>
@@ -451,27 +451,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -881,18 +861,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="71.7109375" customWidth="1"/>
     <col min="3" max="12" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -932,8 +912,11 @@
       <c r="M1" s="1">
         <v>41407</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="1">
+        <v>41408</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -959,7 +942,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -997,7 +980,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1034,8 +1017,11 @@
       <c r="M4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1073,7 +1059,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1111,7 +1097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1149,7 +1135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1187,7 +1173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1225,7 +1211,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1263,7 +1249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1298,7 +1284,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1327,7 +1313,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1362,7 +1348,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1397,7 +1383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1429,7 +1415,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2624,47 +2610,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C9">
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:Z39 H40:H41">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:Y354">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add posibility to choose arguments in selects
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="64">
   <si>
     <t>№</t>
   </si>
@@ -862,7 +862,7 @@
   <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,6 +1095,9 @@
       </c>
       <c r="M6" t="s">
         <v>8</v>
+      </c>
+      <c r="N6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix convertion of conditions from code to visual mode
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="63">
   <si>
     <t>№</t>
   </si>
@@ -351,9 +351,6 @@
   </si>
   <si>
     <t>в селекте не выбираются аргументы</t>
-  </si>
-  <si>
-    <t>is blocked by #54</t>
   </si>
   <si>
     <t>need to add name or number</t>
@@ -454,26 +451,6 @@
   <dxfs count="11">
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -509,6 +486,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -861,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,7 +1856,7 @@
         <v>8</v>
       </c>
       <c r="N30" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -2182,7 +2179,7 @@
         <v>8</v>
       </c>
       <c r="N43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2208,7 +2205,7 @@
         <v>8</v>
       </c>
       <c r="N44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2301,7 +2298,7 @@
         <v>8</v>
       </c>
       <c r="N50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2318,7 +2315,7 @@
         <v>8</v>
       </c>
       <c r="N51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2353,16 +2350,19 @@
       <c r="M54" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M55" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2370,7 +2370,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M56" t="s">
         <v>8</v>
@@ -2629,31 +2629,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:Z39 H40:H41">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:Y354">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix convertion of while statement from code to visual mode
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="62">
   <si>
     <t>№</t>
   </si>
@@ -368,9 +368,6 @@
   if compare(arg1, "!=", arg2):
     pourOut(arg1)
 func0(5)</t>
-  </si>
-  <si>
-    <t>is blocked by#55</t>
   </si>
   <si>
     <t>Не конвертируется в команды, TypeError: (intermediate value).dict is undefined
@@ -859,7 +856,7 @@
   <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+      <selection activeCell="N57" sqref="N57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,7 +2202,7 @@
         <v>8</v>
       </c>
       <c r="N44" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2298,7 +2295,7 @@
         <v>8</v>
       </c>
       <c r="N50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2315,7 +2312,7 @@
         <v>8</v>
       </c>
       <c r="N51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2370,10 +2367,13 @@
         <v>56</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M56" t="s">
         <v>8</v>
+      </c>
+      <c r="N56" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix clone's creation of while and if statements
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="61">
   <si>
     <t>№</t>
   </si>
@@ -330,7 +330,41 @@
     <t>ошибка при вводе корректного каунтера с клавиатуры</t>
   </si>
   <si>
-    <t xml:space="preserve">не конвертируются аргументы функции в каунтере фора:
+    <t>в селекте не выбираются аргументы</t>
+  </si>
+  <si>
+    <t>need to add name or number</t>
+  </si>
+  <si>
+    <t>Некорректно конвертируются условия в команды 
+def func0(arg0):
+  if compare(2, "!=", arg0):
+    if checkFilled(1, "&gt;", 2):
+      sub(1, 2, arg0)
+    else:
+      sub(2, 1, arg0)
+def sub(arg0, arg1, arg2):
+  pour(arg0, arg1)
+  if compare(arg1, "!=", arg2):
+    pourOut(arg1)
+func0(5)</t>
+  </si>
+  <si>
+    <t>Не конвертируется в команды, TypeError: (intermediate value).dict is undefined
+def func0():
+  while objectPosition("wall", "atTheLeft"):
+    forward(1)
+for i in range(3):
+  forward(4)
+forward(1)
+func0()
+if objectPosition("wall", "atTheLeft"):
+  forward(1)
+else:
+  forward(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">некорректный счетчик
 def moveForward():
   while not objectPosition("wall", "inFrontOf"):
     forward(1)
@@ -348,43 +382,6 @@
 right(1)
 solve(32)
 </t>
-  </si>
-  <si>
-    <t>в селекте не выбираются аргументы</t>
-  </si>
-  <si>
-    <t>need to add name or number</t>
-  </si>
-  <si>
-    <t>Некорректно конвертируются условия в команды 
-def func0(arg0):
-  if compare(2, "!=", arg0):
-    if checkFilled(1, "&gt;", 2):
-      sub(1, 2, arg0)
-    else:
-      sub(2, 1, arg0)
-def sub(arg0, arg1, arg2):
-  pour(arg0, arg1)
-  if compare(arg1, "!=", arg2):
-    pourOut(arg1)
-func0(5)</t>
-  </si>
-  <si>
-    <t>Не конвертируется в команды, TypeError: (intermediate value).dict is undefined
-def func0():
-  while objectPosition("wall", "atTheLeft"):
-    forward(1)
-for i in range(3):
-  forward(4)
-forward(1)
-func0()
-if objectPosition("wall", "atTheLeft"):
-  forward(1)
-else:
-  forward(1)</t>
-  </si>
-  <si>
-    <t>is  blocked by #56</t>
   </si>
 </sst>
 </file>
@@ -855,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N57" sqref="N57"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O57" sqref="O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,7 +2173,7 @@
         <v>8</v>
       </c>
       <c r="N43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2295,7 +2292,7 @@
         <v>8</v>
       </c>
       <c r="N50" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2303,7 +2300,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L51" t="s">
         <v>9</v>
@@ -2312,7 +2309,7 @@
         <v>8</v>
       </c>
       <c r="N51" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2342,7 +2339,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M54" t="s">
         <v>8</v>
@@ -2356,7 +2353,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M55" t="s">
         <v>9</v>
@@ -2367,7 +2364,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M56" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
initialize arguments in for statement before starting of its exection
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="61">
   <si>
     <t>№</t>
   </si>
@@ -445,6 +445,26 @@
   <dxfs count="11">
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -480,26 +500,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -850,20 +850,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N103"/>
+  <dimension ref="A1:O103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O57" sqref="O57"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="71.7109375" customWidth="1"/>
     <col min="3" max="12" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -906,8 +906,11 @@
       <c r="N1" s="1">
         <v>41408</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="1">
+        <v>41409</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -933,7 +936,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -971,7 +974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1205,7 +1208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1307,7 +1310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1377,7 +1380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1409,7 +1412,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2264,7 +2267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>49</v>
       </c>
@@ -2278,7 +2281,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
@@ -2295,7 +2298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51</v>
       </c>
@@ -2311,8 +2314,11 @@
       <c r="N51" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>52</v>
       </c>
@@ -2323,7 +2329,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
@@ -2334,7 +2340,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>54</v>
       </c>
@@ -2348,7 +2354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
@@ -2359,7 +2365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>56</v>
       </c>
@@ -2373,42 +2379,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>64</v>
       </c>
@@ -2626,31 +2632,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:Z39 H40:H41">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:Y354">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
proper handle manual changes of counters
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="65">
   <si>
     <t>№</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>функции compare и checkFilled некорректно работают, если передать пустой аргумент в селекте или каунтере</t>
+  </si>
+  <si>
+    <t>если вручную ввести некорректный счетчик, команда выполняется 1 раз</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -459,116 +462,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -979,20 +872,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O102"/>
+  <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P60" sqref="P60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="71.7109375" customWidth="1"/>
     <col min="3" max="14" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1038,8 +931,11 @@
       <c r="O1" s="1">
         <v>41409</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="1">
+        <v>41410</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1068,7 +964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1109,7 +1005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1153,7 +1049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1194,7 +1090,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1238,7 +1134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1279,7 +1175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1320,7 +1216,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1361,7 +1257,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1402,7 +1298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1440,7 +1336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1472,7 +1368,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1510,7 +1406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1548,7 +1444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1583,7 +1479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2537,7 +2433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>49</v>
       </c>
@@ -2554,7 +2450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
@@ -2574,7 +2470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51</v>
       </c>
@@ -2594,7 +2490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>52</v>
       </c>
@@ -2608,7 +2504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
@@ -2621,8 +2517,11 @@
       <c r="O53" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>54</v>
       </c>
@@ -2639,7 +2538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
@@ -2653,7 +2552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>56</v>
       </c>
@@ -2670,7 +2569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>57</v>
       </c>
@@ -2681,7 +2580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>58</v>
       </c>
@@ -2692,7 +2591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>60</v>
       </c>
@@ -2703,27 +2602,33 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>61</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>65</v>
       </c>
@@ -2920,47 +2825,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C9">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:Z39 H40:H41">
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:Y353">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix creation of clones of conditional statements
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P60" sqref="P60"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P61" sqref="P61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,7 +2610,7 @@
         <v>64</v>
       </c>
       <c r="P60" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add verifecation of arguments in pourer's test functions
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="65">
   <si>
     <t>№</t>
   </si>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P61" sqref="P61"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P60" sqref="P60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2579,6 +2579,9 @@
       <c r="O57" t="s">
         <v>8</v>
       </c>
+      <c r="P57" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="58" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -2590,6 +2593,9 @@
       <c r="O58" t="s">
         <v>8</v>
       </c>
+      <c r="P58" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59">
@@ -2601,6 +2607,9 @@
       <c r="O59" t="s">
         <v>8</v>
       </c>
+      <c r="P59" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -2610,7 +2619,7 @@
         <v>64</v>
       </c>
       <c r="P60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add problem stages. don't update command's list during convertion from code to visual mode
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -912,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix removing of function's definitions
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="68">
   <si>
     <t>№</t>
   </si>
@@ -432,6 +432,23 @@
   if objectPosition(arg0, "atTheLeft"):
     forward(arg1)
 func0("Стена", 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">не выполняется и не выдается сообщение об ошибке
+def rotate():
+  if objectPosition("wall", "atTheLeft"):
+    right(1)
+  else:
+    left(1)
+  forward(1)
+def solve(arg0):
+  for i in range(arg0):
+    rotate()
+def solve1(arg0):
+  for i in range(20):
+solve(20)
+solve1(20)
+</t>
   </si>
 </sst>
 </file>
@@ -910,20 +927,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q102"/>
+  <dimension ref="A1:R102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O75" sqref="O75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="71.7109375" customWidth="1"/>
     <col min="3" max="14" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="15" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -975,8 +992,11 @@
       <c r="Q1" s="1">
         <v>41412</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="1">
+        <v>41413</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1005,7 +1025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1046,7 +1066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1090,7 +1110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1131,7 +1151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1175,7 +1195,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1216,7 +1236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1257,7 +1277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1298,7 +1318,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1339,7 +1359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1377,7 +1397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1409,7 +1429,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1447,7 +1467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1485,7 +1505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1520,7 +1540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2474,7 +2494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>49</v>
       </c>
@@ -2491,7 +2511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
@@ -2511,7 +2531,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51</v>
       </c>
@@ -2531,7 +2551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>52</v>
       </c>
@@ -2545,7 +2565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
@@ -2562,7 +2582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>54</v>
       </c>
@@ -2579,7 +2599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
@@ -2593,7 +2613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>56</v>
       </c>
@@ -2610,7 +2630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>57</v>
       </c>
@@ -2624,7 +2644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>58</v>
       </c>
@@ -2638,7 +2658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>60</v>
       </c>
@@ -2652,7 +2672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>61</v>
       </c>
@@ -2663,7 +2683,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>62</v>
       </c>
@@ -2673,8 +2693,11 @@
       <c r="Q61" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>63</v>
       </c>
@@ -2685,12 +2708,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>64</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
add line numbers in ParserErrors. Fixes #12
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O75" sqref="O75"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R64" sqref="R64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2716,7 +2716,7 @@
         <v>67</v>
       </c>
       <c r="R63" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
properly return value in CommandArgumentInput
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="69">
   <si>
     <t>№</t>
   </si>
@@ -449,6 +449,13 @@
 solve(20)
 solve1(20)
 </t>
+  </si>
+  <si>
+    <t>Копируются кавычки в инпуте
+def func0(arg0, arg1):
+  if objectPosition(arg0, "atTheLeft"):
+    forward(arg1)
+func0("Стена", 3)</t>
   </si>
 </sst>
 </file>
@@ -930,7 +937,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R64" sqref="R64"/>
+      <selection activeCell="R63" sqref="R63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2707,6 +2714,9 @@
       <c r="Q62" t="s">
         <v>8</v>
       </c>
+      <c r="R62" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="63" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63">
@@ -2719,9 +2729,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>65</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R64" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
substitute argument's values during execution of commands
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="69">
   <si>
     <t>№</t>
   </si>
@@ -937,7 +937,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R63" sqref="R63"/>
+      <selection activeCell="R48" sqref="R48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,7 +2094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
@@ -2486,8 +2486,11 @@
       <c r="O47" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
       </c>
@@ -2729,7 +2732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
proper check counter value before starting of the execution
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="69">
   <si>
     <t>№</t>
   </si>
@@ -937,7 +937,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R48" sqref="R48"/>
+      <selection activeCell="R61" sqref="R61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2691,6 +2691,9 @@
       </c>
       <c r="P60" t="s">
         <v>8</v>
+      </c>
+      <c r="R60" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix changing of conditional functions and add "pass" statement in empty blocks
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="71">
   <si>
     <t>№</t>
   </si>
@@ -456,6 +456,14 @@
   if objectPosition(arg0, "atTheLeft"):
     forward(arg1)
 func0("Стена", 3)</t>
+  </si>
+  <si>
+    <t>Некорректно выполняется в визуальном режиме
+for i in range(2):
+    pass</t>
+  </si>
+  <si>
+    <t>Падает смена типа условия в теле функции</t>
   </si>
 </sst>
 </file>
@@ -934,20 +942,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R102"/>
+  <dimension ref="A1:S102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R61" sqref="R61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S67" sqref="S67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="14" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="15" max="18" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="18" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1002,8 +1010,11 @@
       <c r="R1" s="1">
         <v>41413</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" s="1">
+        <v>41414</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1031,8 +1042,11 @@
       <c r="O2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1072,8 +1086,11 @@
       <c r="O3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1116,8 +1133,11 @@
       <c r="O4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1157,8 +1177,11 @@
       <c r="O5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1201,8 +1224,11 @@
       <c r="O6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1242,8 +1268,11 @@
       <c r="O7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1283,8 +1312,11 @@
       <c r="O8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1324,8 +1356,11 @@
       <c r="O9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1365,8 +1400,11 @@
       <c r="O10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1403,8 +1441,11 @@
       <c r="O11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1435,8 +1476,11 @@
       <c r="O12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1473,8 +1517,11 @@
       <c r="O13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1511,8 +1558,11 @@
       <c r="O14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1546,8 +1596,11 @@
       <c r="O15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1581,8 +1634,11 @@
       <c r="O16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1616,8 +1672,11 @@
       <c r="O17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1651,8 +1710,11 @@
       <c r="O18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1686,8 +1748,11 @@
       <c r="O19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1721,8 +1786,11 @@
       <c r="O20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1756,8 +1824,11 @@
       <c r="O21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1791,8 +1862,11 @@
       <c r="O22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1823,8 +1897,11 @@
       <c r="O23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1855,8 +1932,11 @@
       <c r="O24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1887,8 +1967,11 @@
       <c r="O25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1919,8 +2002,11 @@
       <c r="O26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1951,8 +2037,11 @@
       <c r="O27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1977,8 +2066,11 @@
       <c r="O28" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2003,8 +2095,11 @@
       <c r="O29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2036,7 +2131,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2065,7 +2160,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2746,82 +2841,94 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>66</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>67</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>78</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>79</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
generate argument values in  function call before checking whether it's finsihed or not (we need to pass arguments to commands in isFinished() to check the correctness of counters)
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="71">
   <si>
     <t>№</t>
   </si>
@@ -944,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S67" sqref="S67"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,6 +2130,9 @@
       <c r="O30" t="s">
         <v>9</v>
       </c>
+      <c r="S30" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -2159,6 +2162,9 @@
       <c r="O31" t="s">
         <v>9</v>
       </c>
+      <c r="S31" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -2188,8 +2194,11 @@
       <c r="O32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2217,8 +2226,11 @@
       <c r="O33" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2246,8 +2258,11 @@
       <c r="O34" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2275,8 +2290,11 @@
       <c r="O35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2304,8 +2322,11 @@
       <c r="O36" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2333,8 +2354,11 @@
       <c r="O37" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2359,8 +2383,11 @@
       <c r="O38" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2385,8 +2412,11 @@
       <c r="O39" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2411,8 +2441,11 @@
       <c r="O40" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2437,8 +2470,11 @@
       <c r="O41" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2463,8 +2499,11 @@
       <c r="O42" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2492,8 +2531,11 @@
       <c r="O43" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2522,7 +2564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
@@ -2548,7 +2590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
@@ -2568,7 +2610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
@@ -2585,7 +2627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
fix execution of commands in block
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="15480" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S52" sqref="S52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2735,7 +2735,7 @@
         <v>9</v>
       </c>
       <c r="S51" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add w/a for execution of empty body in for statement
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S52" sqref="S52"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S66" sqref="S66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2809,7 +2809,7 @@
         <v>9</v>
       </c>
       <c r="S55" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2945,7 +2945,7 @@
         <v>9</v>
       </c>
       <c r="S63" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2970,7 +2970,7 @@
         <v>69</v>
       </c>
       <c r="S65" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
proper update type of condition on changing of its name
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="15480" windowHeight="9120"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="72">
   <si>
     <t>№</t>
   </si>
@@ -958,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T102"/>
+  <dimension ref="A1:U102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T67" sqref="T67"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,9 +969,10 @@
     <col min="2" max="2" width="71.7109375" customWidth="1"/>
     <col min="3" max="18" width="10.140625" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1029,8 +1030,11 @@
       <c r="S1" s="1">
         <v>41414</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U1" s="1">
+        <v>41419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1061,8 +1065,11 @@
       <c r="S2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1105,8 +1112,11 @@
       <c r="S3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1152,8 +1162,11 @@
       <c r="S4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1196,8 +1209,11 @@
       <c r="S5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1243,8 +1259,11 @@
       <c r="S6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1287,8 +1306,11 @@
       <c r="S7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1331,8 +1353,11 @@
       <c r="S8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1375,8 +1400,11 @@
       <c r="S9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1419,8 +1447,11 @@
       <c r="S10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1460,8 +1491,11 @@
       <c r="S11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1495,8 +1529,11 @@
       <c r="S12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1536,8 +1573,11 @@
       <c r="S13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1577,8 +1617,11 @@
       <c r="S14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1615,8 +1658,11 @@
       <c r="S15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1653,8 +1699,11 @@
       <c r="S16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1691,8 +1740,11 @@
       <c r="S17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1729,8 +1781,11 @@
       <c r="S18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1767,8 +1822,11 @@
       <c r="S19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1805,8 +1863,11 @@
       <c r="S20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1843,8 +1904,11 @@
       <c r="S21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1881,8 +1945,11 @@
       <c r="S22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1916,8 +1983,11 @@
       <c r="S23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1951,8 +2021,11 @@
       <c r="S24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1987,7 +2060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2022,7 +2095,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2057,7 +2130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2086,7 +2159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2115,7 +2188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2150,7 +2223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2182,7 +2255,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
don't add function arguments as possible values of condition function name
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="72">
   <si>
     <t>№</t>
   </si>
@@ -961,7 +961,7 @@
   <dimension ref="A1:U102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,6 +2059,9 @@
       <c r="S25" t="s">
         <v>9</v>
       </c>
+      <c r="U25" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -2094,6 +2097,9 @@
       <c r="S26" t="s">
         <v>9</v>
       </c>
+      <c r="U26" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -2129,6 +2135,9 @@
       <c r="S27" t="s">
         <v>9</v>
       </c>
+      <c r="U27" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -2158,6 +2167,9 @@
       <c r="S28" t="s">
         <v>3</v>
       </c>
+      <c r="U28" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -2187,6 +2199,9 @@
       <c r="S29" t="s">
         <v>3</v>
       </c>
+      <c r="U29" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -2222,6 +2237,9 @@
       <c r="S30" t="s">
         <v>9</v>
       </c>
+      <c r="U30" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -2252,6 +2270,9 @@
         <v>9</v>
       </c>
       <c r="S31" t="s">
+        <v>9</v>
+      </c>
+      <c r="U31" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix returning to the previous step
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="71">
   <si>
     <t>№</t>
   </si>
@@ -945,21 +945,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U101"/>
+  <dimension ref="A1:V101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U67" sqref="U67"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="2" max="2" width="87.7109375" customWidth="1"/>
     <col min="3" max="18" width="10.140625" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1020,8 +1020,11 @@
       <c r="U1" s="1">
         <v>41419</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V1" s="1">
+        <v>41429</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1055,8 +1058,11 @@
       <c r="U2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1102,8 +1108,11 @@
       <c r="U3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1152,8 +1161,11 @@
       <c r="U4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1199,8 +1211,11 @@
       <c r="U5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1249,8 +1264,11 @@
       <c r="U6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1296,8 +1314,11 @@
       <c r="U7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1343,8 +1364,11 @@
       <c r="U8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1390,8 +1414,11 @@
       <c r="U9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1437,8 +1464,11 @@
       <c r="U10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1481,8 +1511,11 @@
       <c r="U11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1519,8 +1552,11 @@
       <c r="U12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1563,8 +1599,11 @@
       <c r="U13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1607,8 +1646,11 @@
       <c r="U14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1648,8 +1690,11 @@
       <c r="U15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1689,8 +1734,11 @@
       <c r="U16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1730,8 +1778,11 @@
       <c r="U17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1771,8 +1822,11 @@
       <c r="U18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1812,8 +1866,11 @@
       <c r="U19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1853,8 +1910,11 @@
       <c r="U20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1894,8 +1954,11 @@
       <c r="U21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1935,8 +1998,11 @@
       <c r="U22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1973,8 +2039,11 @@
       <c r="U23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2011,8 +2080,11 @@
       <c r="U24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2049,8 +2121,11 @@
       <c r="U25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2087,8 +2162,11 @@
       <c r="U26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2125,8 +2203,11 @@
       <c r="U27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2157,8 +2238,11 @@
       <c r="U28" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2189,8 +2273,11 @@
       <c r="U29" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2227,8 +2314,11 @@
       <c r="U30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2262,8 +2352,11 @@
       <c r="U31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2297,8 +2390,11 @@
       <c r="U32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2332,8 +2428,11 @@
       <c r="U33" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2367,8 +2466,11 @@
       <c r="U34" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2402,8 +2504,11 @@
       <c r="U35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2437,8 +2542,11 @@
       <c r="U36" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2472,8 +2580,11 @@
       <c r="U37" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2504,8 +2615,11 @@
       <c r="U38" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2536,8 +2650,11 @@
       <c r="U39" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2568,8 +2685,11 @@
       <c r="U40" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2600,8 +2720,11 @@
       <c r="U41" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2632,8 +2755,11 @@
       <c r="U42" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2667,8 +2793,11 @@
       <c r="U43" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2702,8 +2831,11 @@
       <c r="U44" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
@@ -2734,8 +2866,11 @@
       <c r="U45" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
@@ -2760,8 +2895,11 @@
       <c r="U46" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
@@ -2783,8 +2921,11 @@
       <c r="U47" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
       </c>
@@ -2803,8 +2944,11 @@
       <c r="U48" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>49</v>
       </c>
@@ -2826,8 +2970,11 @@
       <c r="U49" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
@@ -2852,8 +2999,11 @@
       <c r="U50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51</v>
       </c>
@@ -2881,8 +3031,11 @@
       <c r="U51" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>52</v>
       </c>
@@ -2901,8 +3054,11 @@
       <c r="U52" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
@@ -2924,8 +3080,11 @@
       <c r="U53" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2947,8 +3106,11 @@
       <c r="U54" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2970,8 +3132,11 @@
       <c r="U55" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>53</v>
       </c>
@@ -2990,8 +3155,11 @@
       <c r="U56" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>53</v>
       </c>
@@ -3010,8 +3178,11 @@
       <c r="U57" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>53</v>
       </c>
@@ -3030,8 +3201,11 @@
       <c r="U58" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>53</v>
       </c>
@@ -3050,8 +3224,11 @@
       <c r="U59" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>53</v>
       </c>
@@ -3070,8 +3247,11 @@
       <c r="U60" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>53</v>
       </c>
@@ -3090,8 +3270,11 @@
       <c r="U61" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>53</v>
       </c>
@@ -3110,8 +3293,11 @@
       <c r="U62" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>53</v>
       </c>
@@ -3127,8 +3313,11 @@
       <c r="U63" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>53</v>
       </c>
@@ -3144,8 +3333,11 @@
       <c r="U64" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>53</v>
       </c>
@@ -3158,8 +3350,11 @@
       <c r="U65" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>53</v>
       </c>
@@ -3175,73 +3370,76 @@
       <c r="U66" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>82</v>
       </c>

</xml_diff>